<commit_message>
recovered glider 386 from deployment 00003. added recovered ingest sheet and updated cal info with recovered date.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL386/Omaha_Cal_Info_CE05MOAS-GL386_00003.xlsx
+++ b/CE05MOAS-GL386/Omaha_Cal_Info_CE05MOAS-GL386_00003.xlsx
@@ -35,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$80</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$321</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +812,9 @@
       <c r="E2" s="6">
         <v>0.94930555555555562</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5">
+        <v>42330</v>
+      </c>
       <c r="G2" s="7" t="s">
         <v>31</v>
       </c>

</xml_diff>